<commit_message>
Deploying to gh-pages from  @ f734ef70b9e267883e6082f402e7b6efcd9f1ae7 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_1-3-1.xlsx
+++ b/assets/excel/2021_1-3-1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15-Uebergreifende-Analysen\Projekte\Integrationsmonitoring_2021\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\NV.Niedersachsen.de\LSN-OG\Hannover\Dez15-Uebergreifende-Analysen\Projekte\Integrationsmonitoring_2021\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4453FC1-90F4-4705-8816-81B7EB02531A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C30BB53-B178-471E-B100-72956E13C64D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{CD3F59CD-FBB8-4114-883D-A6BBE5CD1D50}"/>
   </bookViews>
@@ -295,9 +295,6 @@
     <t xml:space="preserve"> 7 857,0</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <r>
       <t>Tabelle 1.3.1: Menschen mit und ohne Zuwanderungsgeschichte nach Kreisen</t>
     </r>
@@ -311,7 +308,10 @@
     </r>
   </si>
   <si>
-    <t>4) Die Ergebnisse des Mikrozensus 2020 sind unter anderem aufgrund methodischer Effekte im Rahmen einer Neugestaltung der Erhebung sowie insbesondere aufgrund der Folgen der Corona-Pandemie in Ihrer Datenqualität eingeschränkt. Auf die Verwendung dieser Ergebnisse wird daher verzichtet. Weitere Informationen zur methodischen Neugestaltung des Mikrozensus ab 2020 und zu den Auswirkungen der Neugestaltung und der Corona-Krise auf die Ergebnisse des Jahres 2020 finden Sie auf der Informationsseite des Statistischen Bundesamtes: https://www.destatis.de/DE/Themen/Gesellschaft-Umwelt/Bevoelkerung/Haushalte-Familien/Methoden/mikrozensus-2020.html</t>
+    <t>https://www.destatis.de/DE/Themen/Gesellschaft-Umwelt/Bevoelkerung/Haushalte-Familien/Methoden/mikrozensus-2020.html</t>
+  </si>
+  <si>
+    <t>4) Die Ergebnisse des Mikrozensus 2020 sind unter anderem aufgrund methodischer Effekte im Rahmen einer Neugestaltung der Erhebung sowie insbesondere aufgrund der Folgen der Corona-Pandemie in Ihrer Datenqualität eingeschränkt. Auf die Verwendung dieser Ergebnisse wird daher verzichtet. Weitere Informationen zur methodischen Neugestaltung des Mikrozensus ab 2020 und zu den Auswirkungen der Neugestaltung und der Corona-Krise auf die Ergebnisse des Jahres 2020 finden Sie auf der Informationsseite des Statistischen Bundesamtes:</t>
   </si>
 </sst>
 </file>
@@ -618,7 +618,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -752,6 +752,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -779,11 +782,11 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="29">
@@ -1128,9 +1131,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06DBC63E-FF2A-48D5-9066-9477AC3D1A19}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="B1:J490"/>
+  <dimension ref="B1:J491"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A391" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A462" sqref="A462:XFD462"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1160,17 +1165,17 @@
     <row r="4" spans="2:10" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
     </row>
     <row r="7" spans="2:10" ht="33" x14ac:dyDescent="0.25">
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="50" t="s">
+      <c r="D7" s="51" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="9" t="s">
@@ -1193,18 +1198,18 @@
       </c>
     </row>
     <row r="8" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="49"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="52">
+      <c r="C8" s="50"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="53">
         <v>1000</v>
       </c>
-      <c r="F8" s="53"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="55" t="s">
+      <c r="F8" s="54"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="57"/>
     </row>
     <row r="9" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="12">
@@ -1257,8 +1262,8 @@
       <c r="I10" s="37">
         <v>22.8</v>
       </c>
-      <c r="J10" s="36" t="s">
-        <v>77</v>
+      <c r="J10" s="36">
+        <v>20.7</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14340,11 +14345,11 @@
         <v>11.93</v>
       </c>
     </row>
-    <row r="462" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="2:10" s="1" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B462" s="13">
         <v>403</v>
       </c>
-      <c r="C462" s="42" t="s">
+      <c r="C462" s="43" t="s">
         <v>72</v>
       </c>
       <c r="D462" s="15">
@@ -14804,126 +14809,137 @@
         <v>17.239999999999998</v>
       </c>
     </row>
-    <row r="478" spans="2:10" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B478" s="20">
+    <row r="478" spans="2:10" s="34" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B478" s="45">
         <v>0</v>
       </c>
-      <c r="C478" s="19" t="s">
+      <c r="C478" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="D478" s="23">
+      <c r="D478" s="35">
         <v>2011</v>
       </c>
-      <c r="E478" s="24">
+      <c r="E478" s="36">
         <v>7778.2985399999998</v>
       </c>
-      <c r="F478" s="24">
+      <c r="F478" s="36">
         <v>6510.6965700000001</v>
       </c>
-      <c r="G478" s="24">
+      <c r="G478" s="36">
         <v>1267.6019699999999</v>
       </c>
-      <c r="H478" s="24">
+      <c r="H478" s="36">
         <v>83.7</v>
       </c>
-      <c r="I478" s="24">
+      <c r="I478" s="36">
         <v>16.3</v>
       </c>
-      <c r="J478" s="24">
+      <c r="J478" s="36">
         <v>16.3</v>
       </c>
     </row>
     <row r="479" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C479" s="27"/>
     </row>
-    <row r="480" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C480" s="57" t="s">
+    <row r="480" spans="2:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C480" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="D480" s="57"/>
-      <c r="E480" s="57"/>
-      <c r="F480" s="57"/>
-      <c r="G480" s="57"/>
-      <c r="H480" s="57"/>
-      <c r="I480" s="57"/>
-      <c r="J480" s="57"/>
-    </row>
-    <row r="481" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C481" s="58" t="s">
+      <c r="D480" s="48"/>
+      <c r="E480" s="48"/>
+      <c r="F480" s="48"/>
+      <c r="G480" s="48"/>
+      <c r="H480" s="48"/>
+      <c r="I480" s="48"/>
+      <c r="J480" s="48"/>
+    </row>
+    <row r="481" spans="3:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C481" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="D481" s="58"/>
-      <c r="E481" s="58"/>
-      <c r="F481" s="58"/>
-      <c r="G481" s="58"/>
-      <c r="H481" s="58"/>
-      <c r="I481" s="58"/>
-      <c r="J481" s="58"/>
+      <c r="D481" s="59"/>
+      <c r="E481" s="59"/>
+      <c r="F481" s="59"/>
+      <c r="G481" s="59"/>
+      <c r="H481" s="59"/>
+      <c r="I481" s="59"/>
+      <c r="J481" s="59"/>
     </row>
     <row r="482" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C482" s="47" t="s">
+      <c r="C482" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="D482" s="47"/>
-      <c r="E482" s="47"/>
-      <c r="F482" s="47"/>
-      <c r="G482" s="47"/>
-      <c r="H482" s="47"/>
-      <c r="I482" s="47"/>
-      <c r="J482" s="47"/>
-    </row>
-    <row r="483" spans="3:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C483" s="47" t="s">
+      <c r="D482" s="48"/>
+      <c r="E482" s="48"/>
+      <c r="F482" s="48"/>
+      <c r="G482" s="48"/>
+      <c r="H482" s="48"/>
+      <c r="I482" s="48"/>
+      <c r="J482" s="48"/>
+    </row>
+    <row r="483" spans="3:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C483" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="D483" s="47"/>
-      <c r="E483" s="47"/>
-      <c r="F483" s="47"/>
-      <c r="G483" s="47"/>
-      <c r="H483" s="47"/>
-      <c r="I483" s="47"/>
-      <c r="J483" s="47"/>
+      <c r="D483" s="48"/>
+      <c r="E483" s="48"/>
+      <c r="F483" s="48"/>
+      <c r="G483" s="48"/>
+      <c r="H483" s="48"/>
+      <c r="I483" s="48"/>
+      <c r="J483" s="48"/>
     </row>
     <row r="484" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C484" s="44"/>
-      <c r="D484" s="44"/>
-      <c r="E484" s="44"/>
-      <c r="F484" s="44"/>
-      <c r="G484" s="44"/>
-      <c r="H484" s="44"/>
-      <c r="I484" s="44"/>
-      <c r="J484" s="44"/>
+      <c r="C484" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="D484" s="47"/>
+      <c r="E484" s="47"/>
+      <c r="F484" s="47"/>
+      <c r="G484" s="47"/>
+      <c r="H484" s="47"/>
+      <c r="I484" s="47"/>
+      <c r="J484" s="47"/>
     </row>
     <row r="485" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C485" s="28" t="s">
+      <c r="D485" s="44"/>
+      <c r="E485" s="44"/>
+      <c r="F485" s="44"/>
+      <c r="G485" s="44"/>
+      <c r="H485" s="44"/>
+      <c r="I485" s="44"/>
+      <c r="J485" s="44"/>
+    </row>
+    <row r="486" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C486" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="D485" s="29"/>
-      <c r="E485" s="30"/>
-      <c r="F485" s="30"/>
-      <c r="G485" s="30"/>
-      <c r="H485" s="31"/>
-      <c r="I485" s="31"/>
-      <c r="J485"/>
-    </row>
-    <row r="486" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C487" s="28" t="s">
-        <v>61</v>
-      </c>
-    </row>
+      <c r="D486" s="29"/>
+      <c r="E486" s="30"/>
+      <c r="F486" s="30"/>
+      <c r="G486" s="30"/>
+      <c r="H486" s="31"/>
+      <c r="I486" s="31"/>
+      <c r="J486"/>
+    </row>
+    <row r="487" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="488" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C488" s="28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="489" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C489" s="28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="490" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C490" s="28" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="490" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C490" s="41" t="s">
+    <row r="491" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C491" s="41" t="s">
         <v>64</v>
       </c>
     </row>
@@ -14939,7 +14955,8 @@
     <mergeCell ref="C481:J481"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C490" r:id="rId1" xr:uid="{28589D7B-1300-4EC0-9CD3-76B748533734}"/>
+    <hyperlink ref="C491" r:id="rId1" xr:uid="{28589D7B-1300-4EC0-9CD3-76B748533734}"/>
+    <hyperlink ref="C484" r:id="rId2" xr:uid="{1E160BFE-35FA-492D-8918-1FBD59A5DD62}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>